<commit_message>
finalización graficas de inciso a y b
</commit_message>
<xml_diff>
--- a/GraficasProcesos.xlsx
+++ b/GraficasProcesos.xlsx
@@ -8,14 +8,20 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/anahernandez/Documents/3/ALGORITMOS Y DATOS/HDT5/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{896B2273-C33E-2448-A04F-D1D806FC9C4E}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2D483D87-75B2-094C-8CFC-F908BA2B684B}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="13400" yWindow="460" windowWidth="15420" windowHeight="16080" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="IncisoC" sheetId="1" r:id="rId1"/>
     <sheet name="IncisoB" sheetId="2" r:id="rId2"/>
+    <sheet name="IncisoA" sheetId="3" r:id="rId3"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlchart.v1.0" hidden="1">IncisoC!$A$20:$A$24</definedName>
+    <definedName name="_xlchart.v1.1" hidden="1">IncisoC!$B$19</definedName>
+    <definedName name="_xlchart.v1.2" hidden="1">IncisoC!$B$20:$B$24</definedName>
+  </definedNames>
   <calcPr calcId="171027"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -26,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="16">
   <si>
     <t>Memoria a 200</t>
   </si>
@@ -68,6 +74,12 @@
   </si>
   <si>
     <t>Intervalos de 1</t>
+  </si>
+  <si>
+    <t>Tiempo Promedio</t>
+  </si>
+  <si>
+    <t>Intervalos de 10</t>
   </si>
 </sst>
 </file>
@@ -451,6 +463,972 @@
     </c:plotArea>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart10.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>Intervalos de 5</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>IncisoB!$A$3:$A$7</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>25</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>150</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>200</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>IncisoB!$B$3:$B$7</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>21.29</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>40.869999999999997</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>88.91</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>129.97</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>165.81</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-CAAC-0E4B-967F-89542254406E}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="1937175391"/>
+        <c:axId val="1937371311"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="1937175391"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1937371311"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="1937371311"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1937175391"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart11.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="smoothMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>Intervalos de 1</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>IncisoB!$A$22:$A$26</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>25</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>150</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>200</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>IncisoB!$B$22:$B$26</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>26.85</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>42</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>95.99</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>137.35</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>170.29</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-D4BF-8245-B933-80381B85B89D}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="1937090415"/>
+        <c:axId val="2010245423"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="1937090415"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="2010245423"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="2010245423"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1937090415"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart12.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="smoothMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>Procesos vs Tiempo (Intervalos de 10)</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>IncisoA!$A$4:$A$8</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>25</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>150</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>200</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>IncisoA!$B$4:$B$8</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>20.12</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>33.08</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>87.67</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>129.83000000000001</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>163.84</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-6418-F443-868B-A8B4DE8549EC}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="2010707999"/>
+        <c:axId val="2010611583"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="2010707999"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="2010611583"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="2010611583"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="2010707999"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
     <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:spPr>
@@ -3372,6 +4350,126 @@
 </file>
 
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors10.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors11.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors12.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
   <a:schemeClr val="accent2"/>
@@ -4247,6 +5345,1554 @@
 </cs:chartStyle>
 </file>
 
+<file path=xl/charts/style10.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style11.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style12.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
 <file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
   <cs:axisTitle>
@@ -8704,6 +11350,124 @@
 </xdr:wsDr>
 </file>
 
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>133350</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>12700</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>577850</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>88900</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7955B966-47F1-1B49-9B47-657BA5A8B0D9}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>158750</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>50800</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>603250</xdr:colOff>
+      <xdr:row>34</xdr:row>
+      <xdr:rowOff>127000</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="5" name="Chart 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C2FCEBE3-06EF-F54F-8374-AF412ED78BB4}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>400050</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>25400</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>241300</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D53DF02B-8C72-0341-B660-B0DB874ABCA4}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
@@ -9003,7 +11767,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Z38"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="AA47" sqref="AA47"/>
     </sheetView>
   </sheetViews>
@@ -9438,8 +12202,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9C56B7B5-B314-0940-927E-8A70857F2DDA}">
   <dimension ref="A1:B26"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B22" sqref="B22"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E23" sqref="E23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -9561,5 +12325,80 @@
     <mergeCell ref="A20:B20"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6A70239D-A935-1349-86F0-38BED7AC1BD1}">
+  <dimension ref="A2:C8"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B8" sqref="B8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A2" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B2" s="1"/>
+      <c r="C2" s="1"/>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A4">
+        <v>25</v>
+      </c>
+      <c r="B4">
+        <v>20.12</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A5">
+        <v>50</v>
+      </c>
+      <c r="B5">
+        <v>33.08</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A6">
+        <v>100</v>
+      </c>
+      <c r="B6">
+        <v>87.67</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A7">
+        <v>150</v>
+      </c>
+      <c r="B7">
+        <v>129.83000000000001</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A8">
+        <v>200</v>
+      </c>
+      <c r="B8">
+        <v>163.84</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A2:C2"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>